<commit_message>
ASK-41 Fix reading and testing common sections. Fix some benchmarks
</commit_message>
<xml_diff>
--- a/benchmarktests/testdefinitions/Benchmarktest_traject 12-2.xlsx
+++ b/benchmarktests/testdefinitions/Benchmarktest_traject 12-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FF6343-43BE-4E74-A631-55D959824E92}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993D2AB8-A2A2-4CF2-BB57-D9BD80419B16}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="653" firstSheet="1" activeTab="2" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
   </bookViews>
@@ -25,6 +25,9 @@
     <sheet name="Veiligheidsoordeel" sheetId="7" r:id="rId10"/>
     <sheet name="Gecombineerd vakoordeel" sheetId="8" r:id="rId11"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Gecombineerd vakoordeel'!#REF!</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2431,7 +2434,7 @@
   <dimension ref="B1:L135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E106"/>
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2440,6 +2443,7 @@
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2447,7 +2451,7 @@
     </row>
     <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9"/>
-      <c r="C2" s="14"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="69" t="s">
         <v>179</v>
       </c>
@@ -2480,10 +2484,10 @@
       <c r="B3" s="3">
         <v>0</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="7">
         <v>0.16564654600000001</v>
       </c>
-      <c r="D3" s="22" t="str">
+      <c r="D3" s="7" t="str">
         <f t="shared" ref="D3:D34" si="0">IF(COUNTIF(F3:L3,"D")&gt;0,"D",IF(COUNTIF(F3:L3,"-III")&gt;0,"-III",IF(COUNTIF(F3:L3,"-II")&gt;0,"-II",IF(COUNTIF(F3:L3,"-I")&gt;0,"-I",IF(COUNTIF(F3:L3,"+0")&gt;0,"+0",IF(COUNTIF(F3:L3,"+I")&gt;0,"+I",IF(COUNTIF(F3:L3,"+II")&gt;0,"+II",IF(COUNTIF(F3:L3,"+III")&gt;0,"+III",IF(COUNTIF(F3:L3,"ND")&gt;0,"ND","NR")))))))))</f>
         <v>+0</v>
       </c>
@@ -2500,7 +2504,7 @@
         <v>+III</v>
       </c>
       <c r="H3" s="4" t="str">
-        <f t="array" ref="H3">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B3,C3),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H3">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B3,C3),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+II</v>
       </c>
       <c r="I3" s="4" t="str">
@@ -2524,10 +2528,10 @@
       <c r="B4" s="8">
         <v>0.16564654600000001</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="12">
         <v>0.190709198</v>
       </c>
-      <c r="D4" s="23" t="str">
+      <c r="D4" s="12" t="str">
         <f t="shared" si="0"/>
         <v>-III</v>
       </c>
@@ -2544,7 +2548,7 @@
         <v>+III</v>
       </c>
       <c r="H4" s="9" t="str">
-        <f t="array" ref="H4">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B4,C4),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H4">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B4,C4),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+II</v>
       </c>
       <c r="I4" s="9" t="str">
@@ -2568,10 +2572,10 @@
       <c r="B5" s="8">
         <v>0.190709198</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="12">
         <v>0.21</v>
       </c>
-      <c r="D5" s="23" t="str">
+      <c r="D5" s="12" t="str">
         <f t="shared" si="0"/>
         <v>-III</v>
       </c>
@@ -2588,7 +2592,7 @@
         <v>+III</v>
       </c>
       <c r="H5" s="9" t="str">
-        <f t="array" ref="H5">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B5,C5),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H5">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B5,C5),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+II</v>
       </c>
       <c r="I5" s="9" t="str">
@@ -2612,10 +2616,10 @@
       <c r="B6" s="8">
         <v>0.21</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="12">
         <v>0.22009848399999998</v>
       </c>
-      <c r="D6" s="23" t="str">
+      <c r="D6" s="12" t="str">
         <f t="shared" si="0"/>
         <v>-III</v>
       </c>
@@ -2632,7 +2636,7 @@
         <v>+III</v>
       </c>
       <c r="H6" s="9" t="str">
-        <f t="array" ref="H6">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B6,C6),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H6">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B6,C6),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+II</v>
       </c>
       <c r="I6" s="9" t="str">
@@ -2656,10 +2660,10 @@
       <c r="B7" s="8">
         <v>0.22009848399999998</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="12">
         <v>0.23085095799999999</v>
       </c>
-      <c r="D7" s="23" t="str">
+      <c r="D7" s="12" t="str">
         <f t="shared" si="0"/>
         <v>-III</v>
       </c>
@@ -2676,7 +2680,7 @@
         <v>+III</v>
       </c>
       <c r="H7" s="9" t="str">
-        <f t="array" ref="H7">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B7,C7),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H7">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B7,C7),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+II</v>
       </c>
       <c r="I7" s="9" t="str">
@@ -2700,10 +2704,10 @@
       <c r="B8" s="8">
         <v>0.23085095799999999</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="12">
         <v>0.24</v>
       </c>
-      <c r="D8" s="23" t="str">
+      <c r="D8" s="12" t="str">
         <f t="shared" si="0"/>
         <v>-III</v>
       </c>
@@ -2720,7 +2724,7 @@
         <v>+III</v>
       </c>
       <c r="H8" s="9" t="str">
-        <f t="array" ref="H8">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B8,C8),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H8">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B8,C8),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+II</v>
       </c>
       <c r="I8" s="9" t="str">
@@ -2744,10 +2748,10 @@
       <c r="B9" s="8">
         <v>0.24</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="12">
         <v>0.240850958</v>
       </c>
-      <c r="D9" s="23" t="str">
+      <c r="D9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>-III</v>
       </c>
@@ -2764,7 +2768,7 @@
         <v>+III</v>
       </c>
       <c r="H9" s="9" t="str">
-        <f t="array" ref="H9">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B9,C9),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H9">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B9,C9),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+II</v>
       </c>
       <c r="I9" s="9" t="str">
@@ -2788,10 +2792,10 @@
       <c r="B10" s="8">
         <v>0.240850958</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="12">
         <v>0.34</v>
       </c>
-      <c r="D10" s="23" t="str">
+      <c r="D10" s="12" t="str">
         <f t="shared" si="0"/>
         <v>-III</v>
       </c>
@@ -2808,7 +2812,7 @@
         <v>+III</v>
       </c>
       <c r="H10" s="9" t="str">
-        <f t="array" ref="H10">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B10,C10),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H10">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B10,C10),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+II</v>
       </c>
       <c r="I10" s="9" t="str">
@@ -2832,10 +2836,10 @@
       <c r="B11" s="8">
         <v>0.34</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="12">
         <v>0.342187662</v>
       </c>
-      <c r="D11" s="23" t="str">
+      <c r="D11" s="12" t="str">
         <f t="shared" si="0"/>
         <v>-III</v>
       </c>
@@ -2852,7 +2856,7 @@
         <v>+III</v>
       </c>
       <c r="H11" s="9" t="str">
-        <f t="array" ref="H11">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B11,C11),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H11">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B11,C11),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+III</v>
       </c>
       <c r="I11" s="9" t="str">
@@ -2876,10 +2880,10 @@
       <c r="B12" s="8">
         <v>0.342187662</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="12">
         <v>0.91</v>
       </c>
-      <c r="D12" s="23" t="str">
+      <c r="D12" s="12" t="str">
         <f t="shared" si="0"/>
         <v>+III</v>
       </c>
@@ -2896,7 +2900,7 @@
         <v>+III</v>
       </c>
       <c r="H12" s="9" t="str">
-        <f t="array" ref="H12">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B12,C12),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H12">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B12,C12),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+III</v>
       </c>
       <c r="I12" s="9" t="str">
@@ -2920,10 +2924,10 @@
       <c r="B13" s="8">
         <v>0.91</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="12">
         <v>0.995927067</v>
       </c>
-      <c r="D13" s="23" t="str">
+      <c r="D13" s="12" t="str">
         <f t="shared" si="0"/>
         <v>+III</v>
       </c>
@@ -2940,7 +2944,7 @@
         <v>+III</v>
       </c>
       <c r="H13" s="9" t="str">
-        <f t="array" ref="H13">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B13,C13),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H13">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B13,C13),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+III</v>
       </c>
       <c r="I13" s="9" t="str">
@@ -2964,10 +2968,10 @@
       <c r="B14" s="8">
         <v>0.995927067</v>
       </c>
-      <c r="C14" s="9">
-        <v>0.99592706799999997</v>
-      </c>
-      <c r="D14" s="23" t="str">
+      <c r="C14" s="12">
+        <v>1.44</v>
+      </c>
+      <c r="D14" s="12" t="str">
         <f t="shared" si="0"/>
         <v>+I</v>
       </c>
@@ -2984,7 +2988,7 @@
         <v>+III</v>
       </c>
       <c r="H14" s="9" t="str">
-        <f t="array" ref="H14">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B14,C14),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H14">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B14,C14),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+III</v>
       </c>
       <c r="I14" s="9" t="str">
@@ -3006,12 +3010,12 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="8">
-        <v>0.99592706799999997</v>
-      </c>
-      <c r="C15" s="9">
         <v>1.44</v>
       </c>
-      <c r="D15" s="23" t="str">
+      <c r="C15" s="12">
+        <v>1.545093896</v>
+      </c>
+      <c r="D15" s="12" t="str">
         <f t="shared" si="0"/>
         <v>+I</v>
       </c>
@@ -3028,8 +3032,8 @@
         <v>+III</v>
       </c>
       <c r="H15" s="9" t="str">
-        <f t="array" ref="H15">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B15,C15),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="H15">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B15,C15),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+II</v>
       </c>
       <c r="I15" s="9" t="str">
         <f t="array" ref="I15">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B15,C15),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -3050,29 +3054,29 @@
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="8">
-        <v>1.44</v>
-      </c>
-      <c r="C16" s="9">
         <v>1.545093896</v>
       </c>
-      <c r="D16" s="23" t="str">
+      <c r="C16" s="12">
+        <v>1.812946862</v>
+      </c>
+      <c r="D16" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>+I</v>
+        <v>+0</v>
       </c>
       <c r="E16" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>+I</v>
+        <v>+0</v>
       </c>
       <c r="F16" s="9" t="str">
         <f t="array" ref="F16">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B16,C16),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+I</v>
+        <v>+0</v>
       </c>
       <c r="G16" s="9" t="str">
         <f t="array" ref="G16">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B16,C16),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="H16" s="9" t="str">
-        <f t="array" ref="H16">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B16,C16),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H16">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B16,C16),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+II</v>
       </c>
       <c r="I16" s="9" t="str">
@@ -3094,12 +3098,12 @@
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="8">
-        <v>1.545093896</v>
-      </c>
-      <c r="C17" s="9">
         <v>1.812946862</v>
       </c>
-      <c r="D17" s="23" t="str">
+      <c r="C17" s="12">
+        <v>1.96</v>
+      </c>
+      <c r="D17" s="12" t="str">
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
@@ -3116,7 +3120,7 @@
         <v>+III</v>
       </c>
       <c r="H17" s="9" t="str">
-        <f t="array" ref="H17">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B17,C17),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H17">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B17,C17),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+II</v>
       </c>
       <c r="I17" s="9" t="str">
@@ -3138,12 +3142,12 @@
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="8">
-        <v>1.812946862</v>
-      </c>
-      <c r="C18" s="9">
         <v>1.96</v>
       </c>
-      <c r="D18" s="23" t="str">
+      <c r="C18" s="12">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="D18" s="12" t="str">
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
@@ -3160,7 +3164,7 @@
         <v>+III</v>
       </c>
       <c r="H18" s="9" t="str">
-        <f t="array" ref="H18">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B18,C18),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H18">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B18,C18),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+II</v>
       </c>
       <c r="I18" s="9" t="str">
@@ -3182,12 +3186,12 @@
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="8">
-        <v>1.96</v>
-      </c>
-      <c r="C19" s="9">
         <v>2.4900000000000002</v>
       </c>
-      <c r="D19" s="23" t="str">
+      <c r="C19" s="12">
+        <v>2.5196520410000001</v>
+      </c>
+      <c r="D19" s="12" t="str">
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
@@ -3204,8 +3208,8 @@
         <v>+III</v>
       </c>
       <c r="H19" s="9" t="str">
-        <f t="array" ref="H19">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B19,C19),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H19">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B19,C19),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I19" s="9" t="str">
         <f t="array" ref="I19">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B19,C19),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -3226,29 +3230,29 @@
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="8">
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="C20" s="9">
         <v>2.5196520410000001</v>
       </c>
-      <c r="D20" s="23" t="str">
+      <c r="C20" s="12">
+        <v>3.01</v>
+      </c>
+      <c r="D20" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>+0</v>
+        <v>+I</v>
       </c>
       <c r="E20" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>+0</v>
+        <v>+I</v>
       </c>
       <c r="F20" s="9" t="str">
         <f t="array" ref="F20">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B20,C20),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+0</v>
+        <v>+I</v>
       </c>
       <c r="G20" s="9" t="str">
         <f t="array" ref="G20">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B20,C20),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="H20" s="9" t="str">
-        <f t="array" ref="H20">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B20,C20),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H20">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B20,C20),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+III</v>
       </c>
       <c r="I20" s="9" t="str">
@@ -3270,12 +3274,12 @@
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="8">
-        <v>2.5196520410000001</v>
-      </c>
-      <c r="C21" s="9">
         <v>3.01</v>
       </c>
-      <c r="D21" s="23" t="str">
+      <c r="C21" s="12">
+        <v>3.313767881</v>
+      </c>
+      <c r="D21" s="12" t="str">
         <f t="shared" si="0"/>
         <v>+I</v>
       </c>
@@ -3292,8 +3296,8 @@
         <v>+III</v>
       </c>
       <c r="H21" s="9" t="str">
-        <f t="array" ref="H21">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B21,C21),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="H21">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B21,C21),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+II</v>
       </c>
       <c r="I21" s="9" t="str">
         <f t="array" ref="I21">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B21,C21),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -3314,12 +3318,12 @@
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="8">
-        <v>3.01</v>
-      </c>
-      <c r="C22" s="9">
         <v>3.313767881</v>
       </c>
-      <c r="D22" s="23" t="str">
+      <c r="C22" s="12">
+        <v>3.327915993</v>
+      </c>
+      <c r="D22" s="12" t="str">
         <f t="shared" si="0"/>
         <v>+I</v>
       </c>
@@ -3336,7 +3340,7 @@
         <v>+III</v>
       </c>
       <c r="H22" s="9" t="str">
-        <f t="array" ref="H22">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B22,C22),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H22">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B22,C22),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+II</v>
       </c>
       <c r="I22" s="9" t="str">
@@ -3358,29 +3362,29 @@
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="8">
-        <v>3.313767881</v>
-      </c>
-      <c r="C23" s="9">
         <v>3.327915993</v>
       </c>
-      <c r="D23" s="23" t="str">
+      <c r="C23" s="12">
+        <v>3.54</v>
+      </c>
+      <c r="D23" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>+I</v>
+        <v>-II</v>
       </c>
       <c r="E23" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>+I</v>
+        <v>-II</v>
       </c>
       <c r="F23" s="9" t="str">
         <f t="array" ref="F23">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B23,C23),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+I</v>
+        <v>-II</v>
       </c>
       <c r="G23" s="9" t="str">
         <f t="array" ref="G23">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B23,C23),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="H23" s="9" t="str">
-        <f t="array" ref="H23">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B23,C23),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H23">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B23,C23),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+II</v>
       </c>
       <c r="I23" s="9" t="str">
@@ -3402,12 +3406,12 @@
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="8">
-        <v>3.327915993</v>
-      </c>
-      <c r="C24" s="9">
         <v>3.54</v>
       </c>
-      <c r="D24" s="23" t="str">
+      <c r="C24" s="12">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="D24" s="12" t="str">
         <f t="shared" si="0"/>
         <v>-II</v>
       </c>
@@ -3424,7 +3428,7 @@
         <v>+III</v>
       </c>
       <c r="H24" s="9" t="str">
-        <f t="array" ref="H24">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B24,C24),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H24">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B24,C24),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+II</v>
       </c>
       <c r="I24" s="9" t="str">
@@ -3446,12 +3450,12 @@
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="8">
-        <v>3.54</v>
-      </c>
-      <c r="C25" s="9">
         <v>4.0599999999999996</v>
       </c>
-      <c r="D25" s="23" t="str">
+      <c r="C25" s="12">
+        <v>4.3705976250000003</v>
+      </c>
+      <c r="D25" s="12" t="str">
         <f t="shared" si="0"/>
         <v>-II</v>
       </c>
@@ -3468,8 +3472,8 @@
         <v>+III</v>
       </c>
       <c r="H25" s="9" t="str">
-        <f t="array" ref="H25">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B25,C25),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H25">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B25,C25),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I25" s="9" t="str">
         <f t="array" ref="I25">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B25,C25),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -3490,12 +3494,12 @@
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="8">
-        <v>4.0599999999999996</v>
-      </c>
-      <c r="C26" s="9">
         <v>4.3705976250000003</v>
       </c>
-      <c r="D26" s="23" t="str">
+      <c r="C26" s="12">
+        <v>4.58</v>
+      </c>
+      <c r="D26" s="12" t="str">
         <f t="shared" si="0"/>
         <v>-II</v>
       </c>
@@ -3512,7 +3516,7 @@
         <v>+III</v>
       </c>
       <c r="H26" s="9" t="str">
-        <f t="array" ref="H26">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B26,C26),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H26">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B26,C26),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+III</v>
       </c>
       <c r="I26" s="9" t="str">
@@ -3534,12 +3538,12 @@
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="8">
-        <v>4.3705976250000003</v>
-      </c>
-      <c r="C27" s="9">
         <v>4.58</v>
       </c>
-      <c r="D27" s="23" t="str">
+      <c r="C27" s="12">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="D27" s="12" t="str">
         <f t="shared" si="0"/>
         <v>-II</v>
       </c>
@@ -3556,7 +3560,7 @@
         <v>+III</v>
       </c>
       <c r="H27" s="9" t="str">
-        <f t="array" ref="H27">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B27,C27),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H27">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B27,C27),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+III</v>
       </c>
       <c r="I27" s="9" t="str">
@@ -3578,12 +3582,12 @@
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="8">
-        <v>4.58</v>
-      </c>
-      <c r="C28" s="9">
         <v>5.1100000000000003</v>
       </c>
-      <c r="D28" s="23" t="str">
+      <c r="C28" s="12">
+        <v>5.64</v>
+      </c>
+      <c r="D28" s="12" t="str">
         <f t="shared" si="0"/>
         <v>-II</v>
       </c>
@@ -3600,7 +3604,7 @@
         <v>+III</v>
       </c>
       <c r="H28" s="9" t="str">
-        <f t="array" ref="H28">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B28,C28),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H28">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B28,C28),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+III</v>
       </c>
       <c r="I28" s="9" t="str">
@@ -3622,12 +3626,12 @@
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="8">
-        <v>5.1100000000000003</v>
-      </c>
-      <c r="C29" s="9">
         <v>5.64</v>
       </c>
-      <c r="D29" s="23" t="str">
+      <c r="C29" s="12">
+        <v>5.6951114260000004</v>
+      </c>
+      <c r="D29" s="12" t="str">
         <f t="shared" si="0"/>
         <v>-II</v>
       </c>
@@ -3644,7 +3648,7 @@
         <v>+III</v>
       </c>
       <c r="H29" s="9" t="str">
-        <f t="array" ref="H29">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B29,C29),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H29">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B29,C29),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+III</v>
       </c>
       <c r="I29" s="9" t="str">
@@ -3666,12 +3670,12 @@
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="8">
-        <v>5.64</v>
-      </c>
-      <c r="C30" s="9">
         <v>5.6951114260000004</v>
       </c>
-      <c r="D30" s="23" t="str">
+      <c r="C30" s="12">
+        <v>6.24</v>
+      </c>
+      <c r="D30" s="12" t="str">
         <f t="shared" si="0"/>
         <v>-II</v>
       </c>
@@ -3685,10 +3689,10 @@
       </c>
       <c r="G30" s="9" t="str">
         <f t="array" ref="G30">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B30,C30),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <v>+II</v>
       </c>
       <c r="H30" s="9" t="str">
-        <f t="array" ref="H30">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B30,C30),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H30">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B30,C30),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+III</v>
       </c>
       <c r="I30" s="9" t="str">
@@ -3710,12 +3714,12 @@
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="8">
-        <v>5.6951114260000004</v>
-      </c>
-      <c r="C31" s="9">
         <v>6.24</v>
       </c>
-      <c r="D31" s="23" t="str">
+      <c r="C31" s="12">
+        <v>6.84</v>
+      </c>
+      <c r="D31" s="12" t="str">
         <f t="shared" si="0"/>
         <v>-II</v>
       </c>
@@ -3732,7 +3736,7 @@
         <v>+II</v>
       </c>
       <c r="H31" s="9" t="str">
-        <f t="array" ref="H31">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B31,C31),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H31">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B31,C31),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+III</v>
       </c>
       <c r="I31" s="9" t="str">
@@ -3754,12 +3758,12 @@
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="8">
-        <v>6.24</v>
-      </c>
-      <c r="C32" s="9">
         <v>6.84</v>
       </c>
-      <c r="D32" s="23" t="str">
+      <c r="C32" s="12">
+        <v>7.41</v>
+      </c>
+      <c r="D32" s="12" t="str">
         <f t="shared" si="0"/>
         <v>-II</v>
       </c>
@@ -3776,7 +3780,7 @@
         <v>+II</v>
       </c>
       <c r="H32" s="9" t="str">
-        <f t="array" ref="H32">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B32,C32),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H32">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B32,C32),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+III</v>
       </c>
       <c r="I32" s="9" t="str">
@@ -3798,12 +3802,12 @@
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="8">
-        <v>6.84</v>
-      </c>
-      <c r="C33" s="9">
         <v>7.41</v>
       </c>
-      <c r="D33" s="23" t="str">
+      <c r="C33" s="12">
+        <v>7.94</v>
+      </c>
+      <c r="D33" s="12" t="str">
         <f t="shared" si="0"/>
         <v>-II</v>
       </c>
@@ -3820,7 +3824,7 @@
         <v>+II</v>
       </c>
       <c r="H33" s="9" t="str">
-        <f t="array" ref="H33">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B33,C33),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H33">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B33,C33),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+III</v>
       </c>
       <c r="I33" s="9" t="str">
@@ -3842,12 +3846,12 @@
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="8">
-        <v>7.41</v>
-      </c>
-      <c r="C34" s="9">
         <v>7.94</v>
       </c>
-      <c r="D34" s="23" t="str">
+      <c r="C34" s="12">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="D34" s="12" t="str">
         <f t="shared" si="0"/>
         <v>-II</v>
       </c>
@@ -3864,7 +3868,7 @@
         <v>+II</v>
       </c>
       <c r="H34" s="9" t="str">
-        <f t="array" ref="H34">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B34,C34),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H34">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B34,C34),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+III</v>
       </c>
       <c r="I34" s="9" t="str">
@@ -3886,12 +3890,12 @@
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="8">
-        <v>7.94</v>
-      </c>
-      <c r="C35" s="9">
         <v>8.0399999999999991</v>
       </c>
-      <c r="D35" s="23" t="str">
+      <c r="C35" s="12">
+        <v>8.2464557510000009</v>
+      </c>
+      <c r="D35" s="12" t="str">
         <f t="shared" ref="D35:D66" si="2">IF(COUNTIF(F35:L35,"D")&gt;0,"D",IF(COUNTIF(F35:L35,"-III")&gt;0,"-III",IF(COUNTIF(F35:L35,"-II")&gt;0,"-II",IF(COUNTIF(F35:L35,"-I")&gt;0,"-I",IF(COUNTIF(F35:L35,"+0")&gt;0,"+0",IF(COUNTIF(F35:L35,"+I")&gt;0,"+I",IF(COUNTIF(F35:L35,"+II")&gt;0,"+II",IF(COUNTIF(F35:L35,"+III")&gt;0,"+III",IF(COUNTIF(F35:L35,"ND")&gt;0,"ND","NR")))))))))</f>
         <v>-II</v>
       </c>
@@ -3908,7 +3912,7 @@
         <v>+II</v>
       </c>
       <c r="H35" s="9" t="str">
-        <f t="array" ref="H35">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B35,C35),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H35">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B35,C35),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+III</v>
       </c>
       <c r="I35" s="9" t="str">
@@ -3930,29 +3934,29 @@
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="8">
-        <v>8.0399999999999991</v>
-      </c>
-      <c r="C36" s="9">
         <v>8.2464557510000009</v>
       </c>
-      <c r="D36" s="23" t="str">
+      <c r="C36" s="12">
+        <v>8.2505978840000012</v>
+      </c>
+      <c r="D36" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>-II</v>
+        <v>-I</v>
       </c>
       <c r="E36" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>-II</v>
+        <v>-I</v>
       </c>
       <c r="F36" s="9" t="str">
         <f t="array" ref="F36">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B36,C36),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>-II</v>
+        <v>-I</v>
       </c>
       <c r="G36" s="9" t="str">
         <f t="array" ref="G36">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B36,C36),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
         <v>+II</v>
       </c>
       <c r="H36" s="9" t="str">
-        <f t="array" ref="H36">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B36,C36),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H36">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B36,C36),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+III</v>
       </c>
       <c r="I36" s="9" t="str">
@@ -3974,12 +3978,12 @@
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="8">
-        <v>8.2464557510000009</v>
-      </c>
-      <c r="C37" s="9">
         <v>8.2505978840000012</v>
       </c>
-      <c r="D37" s="23" t="str">
+      <c r="C37" s="12">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="D37" s="12" t="str">
         <f t="shared" si="2"/>
         <v>-I</v>
       </c>
@@ -3993,10 +3997,10 @@
       </c>
       <c r="G37" s="9" t="str">
         <f t="array" ref="G37">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B37,C37),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="H37" s="9" t="str">
-        <f t="array" ref="H37">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B37,C37),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H37">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B37,C37),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+III</v>
       </c>
       <c r="I37" s="9" t="str">
@@ -4018,12 +4022,12 @@
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" s="8">
-        <v>8.2505978840000012</v>
-      </c>
-      <c r="C38" s="9">
         <v>8.5399999999999991</v>
       </c>
-      <c r="D38" s="23" t="str">
+      <c r="C38" s="12">
+        <v>8.91</v>
+      </c>
+      <c r="D38" s="12" t="str">
         <f t="shared" si="2"/>
         <v>-I</v>
       </c>
@@ -4040,8 +4044,8 @@
         <v>+III</v>
       </c>
       <c r="H38" s="9" t="str">
-        <f t="array" ref="H38">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B38,C38),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="H38">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B38,C38),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+II</v>
       </c>
       <c r="I38" s="9" t="str">
         <f t="array" ref="I38">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B38,C38),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -4062,12 +4066,12 @@
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" s="8">
-        <v>8.5399999999999991</v>
-      </c>
-      <c r="C39" s="9">
         <v>8.91</v>
       </c>
-      <c r="D39" s="23" t="str">
+      <c r="C39" s="12">
+        <v>8.9463643600000005</v>
+      </c>
+      <c r="D39" s="12" t="str">
         <f t="shared" si="2"/>
         <v>-I</v>
       </c>
@@ -4084,7 +4088,7 @@
         <v>+III</v>
       </c>
       <c r="H39" s="9" t="str">
-        <f t="array" ref="H39">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B39,C39),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H39">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B39,C39),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+II</v>
       </c>
       <c r="I39" s="9" t="str">
@@ -4106,29 +4110,29 @@
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" s="8">
-        <v>8.91</v>
-      </c>
-      <c r="C40" s="9">
         <v>8.9463643600000005</v>
       </c>
-      <c r="D40" s="23" t="str">
+      <c r="C40" s="12">
+        <v>9.2968308060000009</v>
+      </c>
+      <c r="D40" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>-I</v>
+        <v>+II</v>
       </c>
       <c r="E40" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>-I</v>
+        <v>+II</v>
       </c>
       <c r="F40" s="9" t="str">
         <f t="array" ref="F40">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B40,C40),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>-I</v>
+        <v>+II</v>
       </c>
       <c r="G40" s="9" t="str">
         <f t="array" ref="G40">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B40,C40),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="H40" s="9" t="str">
-        <f t="array" ref="H40">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B40,C40),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H40">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B40,C40),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+II</v>
       </c>
       <c r="I40" s="9" t="str">
@@ -4150,12 +4154,12 @@
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" s="8">
-        <v>8.9463643600000005</v>
-      </c>
-      <c r="C41" s="9">
         <v>9.2968308060000009</v>
       </c>
-      <c r="D41" s="23" t="str">
+      <c r="C41" s="12">
+        <v>9.34</v>
+      </c>
+      <c r="D41" s="12" t="str">
         <f t="shared" si="2"/>
         <v>+II</v>
       </c>
@@ -4165,14 +4169,14 @@
       </c>
       <c r="F41" s="9" t="str">
         <f t="array" ref="F41">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B41,C41),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="G41" s="9" t="str">
         <f t="array" ref="G41">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B41,C41),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="H41" s="9" t="str">
-        <f t="array" ref="H41">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B41,C41),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H41">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B41,C41),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+II</v>
       </c>
       <c r="I41" s="9" t="str">
@@ -4194,18 +4198,18 @@
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="8">
-        <v>9.2968308060000009</v>
-      </c>
-      <c r="C42" s="9">
-        <v>9.296830807000001</v>
-      </c>
-      <c r="D42" s="23" t="str">
+        <v>9.34</v>
+      </c>
+      <c r="C42" s="12">
+        <v>9.4600000000000009</v>
+      </c>
+      <c r="D42" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="E42" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="F42" s="9" t="str">
         <f t="array" ref="F42">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B42,C42),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
@@ -4216,8 +4220,8 @@
         <v>+III</v>
       </c>
       <c r="H42" s="9" t="str">
-        <f t="array" ref="H42">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B42,C42),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H42">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B42,C42),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I42" s="9" t="str">
         <f t="array" ref="I42">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B42,C42),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -4238,12 +4242,12 @@
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="8">
-        <v>9.296830807000001</v>
-      </c>
-      <c r="C43" s="9">
-        <v>9.34</v>
-      </c>
-      <c r="D43" s="23" t="str">
+        <v>9.4600000000000009</v>
+      </c>
+      <c r="C43" s="12">
+        <v>9.64</v>
+      </c>
+      <c r="D43" s="12" t="str">
         <f t="shared" si="2"/>
         <v>+II</v>
       </c>
@@ -4260,7 +4264,7 @@
         <v>+III</v>
       </c>
       <c r="H43" s="9" t="str">
-        <f t="array" ref="H43">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B43,C43),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H43">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B43,C43),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+II</v>
       </c>
       <c r="I43" s="9" t="str">
@@ -4282,12 +4286,12 @@
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B44" s="8">
-        <v>9.34</v>
-      </c>
-      <c r="C44" s="9">
-        <v>9.4600000000000009</v>
-      </c>
-      <c r="D44" s="23" t="str">
+        <v>9.64</v>
+      </c>
+      <c r="C44" s="12">
+        <v>9.76</v>
+      </c>
+      <c r="D44" s="12" t="str">
         <f t="shared" si="2"/>
         <v>+II</v>
       </c>
@@ -4304,7 +4308,7 @@
         <v>+III</v>
       </c>
       <c r="H44" s="9" t="str">
-        <f t="array" ref="H44">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B44,C44),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <f t="array" ref="H44">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B44,C44),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
         <v>+II</v>
       </c>
       <c r="I44" s="9" t="str">
@@ -4326,18 +4330,18 @@
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" s="8">
-        <v>9.4600000000000009</v>
-      </c>
-      <c r="C45" s="9">
-        <v>9.64</v>
-      </c>
-      <c r="D45" s="23" t="str">
+        <v>9.76</v>
+      </c>
+      <c r="C45" s="12">
+        <v>9.7975727730000006</v>
+      </c>
+      <c r="D45" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="E45" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="F45" s="9" t="str">
         <f t="array" ref="F45">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B45,C45),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
@@ -4348,8 +4352,8 @@
         <v>+III</v>
       </c>
       <c r="H45" s="9" t="str">
-        <f t="array" ref="H45">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B45,C45),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H45">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B45,C45),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I45" s="9" t="str">
         <f t="array" ref="I45">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B45,C45),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -4370,30 +4374,30 @@
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B46" s="8">
-        <v>9.64</v>
-      </c>
-      <c r="C46" s="9">
-        <v>9.76</v>
-      </c>
-      <c r="D46" s="23" t="str">
+        <v>9.7975727730000006</v>
+      </c>
+      <c r="C46" s="12">
+        <v>10.01</v>
+      </c>
+      <c r="D46" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>+II</v>
+        <v>-II</v>
       </c>
       <c r="E46" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>+II</v>
+        <v>-II</v>
       </c>
       <c r="F46" s="9" t="str">
         <f t="array" ref="F46">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B46,C46),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <v>-II</v>
       </c>
       <c r="G46" s="9" t="str">
         <f t="array" ref="G46">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B46,C46),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="H46" s="9" t="str">
-        <f t="array" ref="H46">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B46,C46),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H46">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B46,C46),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I46" s="9" t="str">
         <f t="array" ref="I46">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B46,C46),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -4414,30 +4418,30 @@
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" s="8">
-        <v>9.76</v>
-      </c>
-      <c r="C47" s="9">
-        <v>9.7975727730000006</v>
-      </c>
-      <c r="D47" s="23" t="str">
+        <v>10.01</v>
+      </c>
+      <c r="C47" s="12">
+        <v>10.59</v>
+      </c>
+      <c r="D47" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>+II</v>
+        <v>-II</v>
       </c>
       <c r="E47" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>+II</v>
+        <v>-II</v>
       </c>
       <c r="F47" s="9" t="str">
         <f t="array" ref="F47">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B47,C47),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <v>-II</v>
       </c>
       <c r="G47" s="9" t="str">
         <f t="array" ref="G47">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B47,C47),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="H47" s="9" t="str">
-        <f t="array" ref="H47">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B47,C47),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H47">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B47,C47),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I47" s="9" t="str">
         <f t="array" ref="I47">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B47,C47),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -4458,12 +4462,12 @@
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B48" s="8">
-        <v>9.7975727730000006</v>
-      </c>
-      <c r="C48" s="9">
-        <v>9.7975727740000007</v>
-      </c>
-      <c r="D48" s="23" t="str">
+        <v>10.59</v>
+      </c>
+      <c r="C48" s="12">
+        <v>11.11</v>
+      </c>
+      <c r="D48" s="12" t="str">
         <f t="shared" si="2"/>
         <v>-II</v>
       </c>
@@ -4480,8 +4484,8 @@
         <v>+III</v>
       </c>
       <c r="H48" s="9" t="str">
-        <f t="array" ref="H48">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B48,C48),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H48">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B48,C48),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I48" s="9" t="str">
         <f t="array" ref="I48">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B48,C48),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -4502,12 +4506,12 @@
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B49" s="8">
-        <v>9.7975727740000007</v>
-      </c>
-      <c r="C49" s="9">
-        <v>10.01</v>
-      </c>
-      <c r="D49" s="23" t="str">
+        <v>11.11</v>
+      </c>
+      <c r="C49" s="12">
+        <v>11.64</v>
+      </c>
+      <c r="D49" s="12" t="str">
         <f t="shared" si="2"/>
         <v>-II</v>
       </c>
@@ -4524,8 +4528,8 @@
         <v>+III</v>
       </c>
       <c r="H49" s="9" t="str">
-        <f t="array" ref="H49">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B49,C49),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H49">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B49,C49),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I49" s="9" t="str">
         <f t="array" ref="I49">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B49,C49),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -4546,12 +4550,12 @@
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B50" s="8">
-        <v>10.01</v>
-      </c>
-      <c r="C50" s="9">
-        <v>10.59</v>
-      </c>
-      <c r="D50" s="23" t="str">
+        <v>11.64</v>
+      </c>
+      <c r="C50" s="12">
+        <v>12.16</v>
+      </c>
+      <c r="D50" s="12" t="str">
         <f t="shared" si="2"/>
         <v>-II</v>
       </c>
@@ -4568,8 +4572,8 @@
         <v>+III</v>
       </c>
       <c r="H50" s="9" t="str">
-        <f t="array" ref="H50">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B50,C50),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H50">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B50,C50),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I50" s="9" t="str">
         <f t="array" ref="I50">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B50,C50),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -4590,12 +4594,12 @@
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" s="8">
-        <v>10.59</v>
-      </c>
-      <c r="C51" s="9">
-        <v>11.11</v>
-      </c>
-      <c r="D51" s="23" t="str">
+        <v>12.16</v>
+      </c>
+      <c r="C51" s="12">
+        <v>12.69</v>
+      </c>
+      <c r="D51" s="12" t="str">
         <f t="shared" si="2"/>
         <v>-II</v>
       </c>
@@ -4612,8 +4616,8 @@
         <v>+III</v>
       </c>
       <c r="H51" s="9" t="str">
-        <f t="array" ref="H51">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B51,C51),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H51">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B51,C51),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I51" s="9" t="str">
         <f t="array" ref="I51">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B51,C51),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -4634,12 +4638,12 @@
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" s="8">
-        <v>11.11</v>
-      </c>
-      <c r="C52" s="9">
-        <v>11.64</v>
-      </c>
-      <c r="D52" s="23" t="str">
+        <v>12.69</v>
+      </c>
+      <c r="C52" s="12">
+        <v>13.19</v>
+      </c>
+      <c r="D52" s="12" t="str">
         <f t="shared" si="2"/>
         <v>-II</v>
       </c>
@@ -4656,8 +4660,8 @@
         <v>+III</v>
       </c>
       <c r="H52" s="9" t="str">
-        <f t="array" ref="H52">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B52,C52),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H52">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B52,C52),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I52" s="9" t="str">
         <f t="array" ref="I52">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B52,C52),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -4678,12 +4682,12 @@
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B53" s="8">
-        <v>11.64</v>
-      </c>
-      <c r="C53" s="9">
-        <v>12.16</v>
-      </c>
-      <c r="D53" s="23" t="str">
+        <v>13.19</v>
+      </c>
+      <c r="C53" s="12">
+        <v>13.197809816000001</v>
+      </c>
+      <c r="D53" s="12" t="str">
         <f t="shared" si="2"/>
         <v>-II</v>
       </c>
@@ -4700,8 +4704,8 @@
         <v>+III</v>
       </c>
       <c r="H53" s="9" t="str">
-        <f t="array" ref="H53">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B53,C53),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H53">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B53,C53),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I53" s="9" t="str">
         <f t="array" ref="I53">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B53,C53),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -4722,30 +4726,30 @@
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B54" s="8">
-        <v>12.16</v>
-      </c>
-      <c r="C54" s="9">
-        <v>12.69</v>
-      </c>
-      <c r="D54" s="23" t="str">
+        <v>13.197809816000001</v>
+      </c>
+      <c r="C54" s="12">
+        <v>13.46</v>
+      </c>
+      <c r="D54" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="E54" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="F54" s="9" t="str">
         <f t="array" ref="F54">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B54,C54),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="G54" s="9" t="str">
         <f t="array" ref="G54">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B54,C54),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="H54" s="9" t="str">
-        <f t="array" ref="H54">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B54,C54),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H54">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B54,C54),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I54" s="9" t="str">
         <f t="array" ref="I54">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B54,C54),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -4766,30 +4770,30 @@
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B55" s="8">
-        <v>12.69</v>
-      </c>
-      <c r="C55" s="9">
-        <v>13.19</v>
-      </c>
-      <c r="D55" s="23" t="str">
+        <v>13.46</v>
+      </c>
+      <c r="C55" s="12">
+        <v>13.84</v>
+      </c>
+      <c r="D55" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="E55" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="F55" s="9" t="str">
         <f t="array" ref="F55">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B55,C55),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="G55" s="9" t="str">
         <f t="array" ref="G55">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B55,C55),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="H55" s="9" t="str">
-        <f t="array" ref="H55">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B55,C55),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H55">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B55,C55),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I55" s="9" t="str">
         <f t="array" ref="I55">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B55,C55),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -4810,30 +4814,30 @@
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B56" s="8">
-        <v>13.19</v>
-      </c>
-      <c r="C56" s="9">
-        <v>13.197809816000001</v>
-      </c>
-      <c r="D56" s="23" t="str">
+        <v>13.84</v>
+      </c>
+      <c r="C56" s="12">
+        <v>14.06</v>
+      </c>
+      <c r="D56" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="E56" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="F56" s="9" t="str">
         <f t="array" ref="F56">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B56,C56),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="G56" s="9" t="str">
         <f t="array" ref="G56">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B56,C56),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="H56" s="9" t="str">
-        <f t="array" ref="H56">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B56,C56),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H56">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B56,C56),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I56" s="9" t="str">
         <f t="array" ref="I56">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B56,C56),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -4854,12 +4858,12 @@
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B57" s="8">
-        <v>13.197809816000001</v>
-      </c>
-      <c r="C57" s="9">
-        <v>13.197809817000001</v>
-      </c>
-      <c r="D57" s="23" t="str">
+        <v>14.06</v>
+      </c>
+      <c r="C57" s="12">
+        <v>14.104461709000001</v>
+      </c>
+      <c r="D57" s="12" t="str">
         <f t="shared" si="2"/>
         <v>+0</v>
       </c>
@@ -4876,8 +4880,8 @@
         <v>+III</v>
       </c>
       <c r="H57" s="9" t="str">
-        <f t="array" ref="H57">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B57,C57),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H57">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B57,C57),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I57" s="9" t="str">
         <f t="array" ref="I57">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B57,C57),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -4898,30 +4902,30 @@
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B58" s="8">
-        <v>13.197809817000001</v>
-      </c>
-      <c r="C58" s="9">
-        <v>13.46</v>
-      </c>
-      <c r="D58" s="23" t="str">
+        <v>14.104461709000001</v>
+      </c>
+      <c r="C58" s="12">
+        <v>14.19</v>
+      </c>
+      <c r="D58" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>+0</v>
+        <v>-II</v>
       </c>
       <c r="E58" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>+0</v>
+        <v>-II</v>
       </c>
       <c r="F58" s="9" t="str">
         <f t="array" ref="F58">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B58,C58),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+0</v>
+        <v>-II</v>
       </c>
       <c r="G58" s="9" t="str">
         <f t="array" ref="G58">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B58,C58),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <v>+II</v>
       </c>
       <c r="H58" s="9" t="str">
-        <f t="array" ref="H58">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B58,C58),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H58">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B58,C58),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I58" s="9" t="str">
         <f t="array" ref="I58">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B58,C58),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -4942,30 +4946,30 @@
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B59" s="8">
-        <v>13.46</v>
-      </c>
-      <c r="C59" s="9">
-        <v>13.84</v>
-      </c>
-      <c r="D59" s="23" t="str">
+        <v>14.19</v>
+      </c>
+      <c r="C59" s="12">
+        <v>14.49</v>
+      </c>
+      <c r="D59" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>+0</v>
+        <v>-II</v>
       </c>
       <c r="E59" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>+0</v>
+        <v>-II</v>
       </c>
       <c r="F59" s="9" t="str">
         <f t="array" ref="F59">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B59,C59),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+0</v>
+        <v>-II</v>
       </c>
       <c r="G59" s="9" t="str">
         <f t="array" ref="G59">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B59,C59),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <v>+II</v>
       </c>
       <c r="H59" s="9" t="str">
-        <f t="array" ref="H59">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B59,C59),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H59">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B59,C59),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I59" s="9" t="str">
         <f t="array" ref="I59">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B59,C59),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -4986,30 +4990,30 @@
     </row>
     <row r="60" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B60" s="8">
-        <v>13.84</v>
-      </c>
-      <c r="C60" s="9">
-        <v>14.06</v>
-      </c>
-      <c r="D60" s="23" t="str">
+        <v>14.49</v>
+      </c>
+      <c r="C60" s="12">
+        <v>15.02</v>
+      </c>
+      <c r="D60" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>+0</v>
+        <v>-II</v>
       </c>
       <c r="E60" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>+0</v>
+        <v>-II</v>
       </c>
       <c r="F60" s="9" t="str">
         <f t="array" ref="F60">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B60,C60),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+0</v>
+        <v>-II</v>
       </c>
       <c r="G60" s="9" t="str">
         <f t="array" ref="G60">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B60,C60),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <v>+II</v>
       </c>
       <c r="H60" s="9" t="str">
-        <f t="array" ref="H60">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B60,C60),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H60">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B60,C60),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I60" s="9" t="str">
         <f t="array" ref="I60">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B60,C60),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5030,30 +5034,30 @@
     </row>
     <row r="61" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B61" s="8">
-        <v>14.06</v>
-      </c>
-      <c r="C61" s="9">
-        <v>14.104461709000001</v>
-      </c>
-      <c r="D61" s="23" t="str">
+        <v>15.02</v>
+      </c>
+      <c r="C61" s="12">
+        <v>15.54</v>
+      </c>
+      <c r="D61" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>+0</v>
+        <v>-II</v>
       </c>
       <c r="E61" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>+0</v>
+        <v>-II</v>
       </c>
       <c r="F61" s="9" t="str">
         <f t="array" ref="F61">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B61,C61),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+0</v>
+        <v>-II</v>
       </c>
       <c r="G61" s="9" t="str">
         <f t="array" ref="G61">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B61,C61),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <v>+II</v>
       </c>
       <c r="H61" s="9" t="str">
-        <f t="array" ref="H61">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B61,C61),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H61">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B61,C61),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I61" s="9" t="str">
         <f t="array" ref="I61">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B61,C61),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5074,12 +5078,12 @@
     </row>
     <row r="62" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B62" s="8">
-        <v>14.104461709000001</v>
-      </c>
-      <c r="C62" s="9">
-        <v>14.104461710000001</v>
-      </c>
-      <c r="D62" s="23" t="str">
+        <v>15.54</v>
+      </c>
+      <c r="C62" s="12">
+        <v>16.059999999999999</v>
+      </c>
+      <c r="D62" s="12" t="str">
         <f t="shared" si="2"/>
         <v>-II</v>
       </c>
@@ -5093,11 +5097,11 @@
       </c>
       <c r="G62" s="9" t="str">
         <f t="array" ref="G62">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B62,C62),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <v>+II</v>
       </c>
       <c r="H62" s="9" t="str">
-        <f t="array" ref="H62">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B62,C62),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H62">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B62,C62),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I62" s="9" t="str">
         <f t="array" ref="I62">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B62,C62),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5118,12 +5122,12 @@
     </row>
     <row r="63" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B63" s="8">
-        <v>14.104461710000001</v>
-      </c>
-      <c r="C63" s="9">
-        <v>14.19</v>
-      </c>
-      <c r="D63" s="23" t="str">
+        <v>16.059999999999999</v>
+      </c>
+      <c r="C63" s="12">
+        <v>16.59</v>
+      </c>
+      <c r="D63" s="12" t="str">
         <f t="shared" si="2"/>
         <v>-II</v>
       </c>
@@ -5140,8 +5144,8 @@
         <v>+II</v>
       </c>
       <c r="H63" s="9" t="str">
-        <f t="array" ref="H63">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B63,C63),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H63">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B63,C63),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I63" s="9" t="str">
         <f t="array" ref="I63">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B63,C63),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5162,12 +5166,12 @@
     </row>
     <row r="64" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B64" s="8">
-        <v>14.19</v>
-      </c>
-      <c r="C64" s="9">
-        <v>14.49</v>
-      </c>
-      <c r="D64" s="23" t="str">
+        <v>16.59</v>
+      </c>
+      <c r="C64" s="12">
+        <v>16.652344551000002</v>
+      </c>
+      <c r="D64" s="12" t="str">
         <f t="shared" si="2"/>
         <v>-II</v>
       </c>
@@ -5184,8 +5188,8 @@
         <v>+II</v>
       </c>
       <c r="H64" s="9" t="str">
-        <f t="array" ref="H64">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B64,C64),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H64">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B64,C64),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I64" s="9" t="str">
         <f t="array" ref="I64">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B64,C64),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5206,12 +5210,12 @@
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B65" s="8">
-        <v>14.49</v>
-      </c>
-      <c r="C65" s="9">
-        <v>15.02</v>
-      </c>
-      <c r="D65" s="23" t="str">
+        <v>16.652344551000002</v>
+      </c>
+      <c r="C65" s="12">
+        <v>16.656083170000002</v>
+      </c>
+      <c r="D65" s="12" t="str">
         <f t="shared" si="2"/>
         <v>-II</v>
       </c>
@@ -5225,11 +5229,11 @@
       </c>
       <c r="G65" s="9" t="str">
         <f t="array" ref="G65">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B65,C65),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="H65" s="9" t="str">
-        <f t="array" ref="H65">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B65,C65),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H65">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B65,C65),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I65" s="9" t="str">
         <f t="array" ref="I65">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B65,C65),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5250,30 +5254,30 @@
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B66" s="8">
-        <v>15.02</v>
-      </c>
-      <c r="C66" s="9">
-        <v>15.54</v>
-      </c>
-      <c r="D66" s="23" t="str">
+        <v>16.656083170000002</v>
+      </c>
+      <c r="C66" s="12">
+        <v>17.11</v>
+      </c>
+      <c r="D66" s="12" t="str">
         <f t="shared" si="2"/>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="E66" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="F66" s="9" t="str">
         <f t="array" ref="F66">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B66,C66),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="G66" s="9" t="str">
         <f t="array" ref="G66">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B66,C66),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="H66" s="9" t="str">
-        <f t="array" ref="H66">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B66,C66),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H66">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B66,C66),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I66" s="9" t="str">
         <f t="array" ref="I66">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B66,C66),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5294,30 +5298,30 @@
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B67" s="8">
-        <v>15.54</v>
-      </c>
-      <c r="C67" s="9">
-        <v>16.059999999999999</v>
-      </c>
-      <c r="D67" s="23" t="str">
+        <v>17.11</v>
+      </c>
+      <c r="C67" s="12">
+        <v>17.155520158000002</v>
+      </c>
+      <c r="D67" s="12" t="str">
         <f t="shared" ref="D67:D98" si="4">IF(COUNTIF(F67:L67,"D")&gt;0,"D",IF(COUNTIF(F67:L67,"-III")&gt;0,"-III",IF(COUNTIF(F67:L67,"-II")&gt;0,"-II",IF(COUNTIF(F67:L67,"-I")&gt;0,"-I",IF(COUNTIF(F67:L67,"+0")&gt;0,"+0",IF(COUNTIF(F67:L67,"+I")&gt;0,"+I",IF(COUNTIF(F67:L67,"+II")&gt;0,"+II",IF(COUNTIF(F67:L67,"+III")&gt;0,"+III",IF(COUNTIF(F67:L67,"ND")&gt;0,"ND","NR")))))))))</f>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="E67" s="23" t="str">
         <f t="shared" ref="E67:E98" si="5">IF(COUNTIF(F67:L67,"-III")&gt;0,"-III",IF(COUNTIF(F67:L67,"-II")&gt;0,"-II",IF(COUNTIF(F67:L67,"-I")&gt;0,"-I",IF(COUNTIF(F67:L67,"+0")&gt;0,"+0",IF(COUNTIF(F67:L67,"+I")&gt;0,"+I",IF(COUNTIF(F67:L67,"+II")&gt;0,"+II",IF(COUNTIF(F67:L67,"+III")&gt;0,"+III",IF(COUNTIF(F67:L67,"ND")&gt;0,"ND","NR"))))))))</f>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="F67" s="9" t="str">
         <f t="array" ref="F67">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B67,C67),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="G67" s="9" t="str">
         <f t="array" ref="G67">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B67,C67),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="H67" s="9" t="str">
-        <f t="array" ref="H67">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B67,C67),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H67">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B67,C67),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I67" s="9" t="str">
         <f t="array" ref="I67">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B67,C67),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5338,30 +5342,30 @@
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B68" s="8">
-        <v>16.059999999999999</v>
-      </c>
-      <c r="C68" s="9">
-        <v>16.59</v>
-      </c>
-      <c r="D68" s="23" t="str">
+        <v>17.155520158000002</v>
+      </c>
+      <c r="C68" s="12">
+        <v>17.71</v>
+      </c>
+      <c r="D68" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="E68" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="F68" s="9" t="str">
         <f t="array" ref="F68">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B68,C68),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="G68" s="9" t="str">
         <f t="array" ref="G68">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B68,C68),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="H68" s="9" t="str">
-        <f t="array" ref="H68">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B68,C68),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H68">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B68,C68),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I68" s="9" t="str">
         <f t="array" ref="I68">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B68,C68),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5382,30 +5386,30 @@
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B69" s="8">
-        <v>16.59</v>
-      </c>
-      <c r="C69" s="9">
-        <v>16.652344551000002</v>
-      </c>
-      <c r="D69" s="23" t="str">
+        <v>17.71</v>
+      </c>
+      <c r="C69" s="12">
+        <v>17.802401842000002</v>
+      </c>
+      <c r="D69" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="E69" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="F69" s="9" t="str">
         <f t="array" ref="F69">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B69,C69),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="G69" s="9" t="str">
         <f t="array" ref="G69">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B69,C69),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="H69" s="9" t="str">
-        <f t="array" ref="H69">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B69,C69),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H69">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B69,C69),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I69" s="9" t="str">
         <f t="array" ref="I69">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B69,C69),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5426,30 +5430,30 @@
     </row>
     <row r="70" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B70" s="8">
-        <v>16.652344551000002</v>
-      </c>
-      <c r="C70" s="9">
-        <v>16.656083170000002</v>
-      </c>
-      <c r="D70" s="23" t="str">
+        <v>17.802401842000002</v>
+      </c>
+      <c r="C70" s="12">
+        <v>17.802979463</v>
+      </c>
+      <c r="D70" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="E70" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="F70" s="9" t="str">
         <f t="array" ref="F70">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B70,C70),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="G70" s="9" t="str">
         <f t="array" ref="G70">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B70,C70),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="H70" s="9" t="str">
-        <f t="array" ref="H70">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B70,C70),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H70">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B70,C70),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I70" s="9" t="str">
         <f t="array" ref="I70">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B70,C70),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5470,30 +5474,30 @@
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B71" s="8">
-        <v>16.656083170000002</v>
-      </c>
-      <c r="C71" s="9">
-        <v>17.11</v>
-      </c>
-      <c r="D71" s="23" t="str">
+        <v>17.802979463</v>
+      </c>
+      <c r="C71" s="12">
+        <v>17.809999999999999</v>
+      </c>
+      <c r="D71" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>+0</v>
+        <v>-III</v>
       </c>
       <c r="E71" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>+0</v>
+        <v>-III</v>
       </c>
       <c r="F71" s="9" t="str">
         <f t="array" ref="F71">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B71,C71),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+0</v>
+        <v>-III</v>
       </c>
       <c r="G71" s="9" t="str">
         <f t="array" ref="G71">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B71,C71),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="H71" s="9" t="str">
-        <f t="array" ref="H71">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B71,C71),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H71">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B71,C71),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I71" s="9" t="str">
         <f t="array" ref="I71">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B71,C71),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5514,30 +5518,30 @@
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B72" s="8">
-        <v>17.11</v>
-      </c>
-      <c r="C72" s="9">
-        <v>17.155520158000002</v>
-      </c>
-      <c r="D72" s="23" t="str">
+        <v>17.809999999999999</v>
+      </c>
+      <c r="C72" s="12">
+        <v>17.850000000000001</v>
+      </c>
+      <c r="D72" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>+0</v>
+        <v>-III</v>
       </c>
       <c r="E72" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>+0</v>
+        <v>-III</v>
       </c>
       <c r="F72" s="9" t="str">
         <f t="array" ref="F72">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B72,C72),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+0</v>
+        <v>-III</v>
       </c>
       <c r="G72" s="9" t="str">
         <f t="array" ref="G72">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B72,C72),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="H72" s="9" t="str">
-        <f t="array" ref="H72">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B72,C72),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H72">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B72,C72),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I72" s="9" t="str">
         <f t="array" ref="I72">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B72,C72),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5558,30 +5562,30 @@
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B73" s="8">
-        <v>17.155520158000002</v>
-      </c>
-      <c r="C73" s="9">
-        <v>17.71</v>
-      </c>
-      <c r="D73" s="23" t="str">
+        <v>17.850000000000001</v>
+      </c>
+      <c r="C73" s="12">
+        <v>17.91</v>
+      </c>
+      <c r="D73" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>+0</v>
+        <v>-III</v>
       </c>
       <c r="E73" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>+0</v>
+        <v>-III</v>
       </c>
       <c r="F73" s="9" t="str">
         <f t="array" ref="F73">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B73,C73),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+0</v>
+        <v>-III</v>
       </c>
       <c r="G73" s="9" t="str">
         <f t="array" ref="G73">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B73,C73),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="H73" s="9" t="str">
-        <f t="array" ref="H73">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B73,C73),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H73">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B73,C73),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I73" s="9" t="str">
         <f t="array" ref="I73">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B73,C73),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5602,30 +5606,30 @@
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B74" s="8">
-        <v>17.71</v>
-      </c>
-      <c r="C74" s="9">
-        <v>17.802401842000002</v>
-      </c>
-      <c r="D74" s="23" t="str">
+        <v>17.91</v>
+      </c>
+      <c r="C74" s="12">
+        <v>18.29</v>
+      </c>
+      <c r="D74" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>+0</v>
+        <v>-III</v>
       </c>
       <c r="E74" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>+0</v>
+        <v>-III</v>
       </c>
       <c r="F74" s="9" t="str">
         <f t="array" ref="F74">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B74,C74),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+0</v>
+        <v>-III</v>
       </c>
       <c r="G74" s="9" t="str">
         <f t="array" ref="G74">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B74,C74),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="H74" s="9" t="str">
-        <f t="array" ref="H74">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B74,C74),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H74">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B74,C74),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I74" s="9" t="str">
         <f t="array" ref="I74">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B74,C74),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5646,30 +5650,30 @@
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B75" s="8">
-        <v>17.802401842000002</v>
-      </c>
-      <c r="C75" s="9">
-        <v>17.802979463</v>
-      </c>
-      <c r="D75" s="23" t="str">
+        <v>18.29</v>
+      </c>
+      <c r="C75" s="12">
+        <v>18.48</v>
+      </c>
+      <c r="D75" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>+0</v>
+        <v>-III</v>
       </c>
       <c r="E75" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>+0</v>
+        <v>-III</v>
       </c>
       <c r="F75" s="9" t="str">
         <f t="array" ref="F75">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B75,C75),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+0</v>
+        <v>-III</v>
       </c>
       <c r="G75" s="9" t="str">
         <f t="array" ref="G75">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B75,C75),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="H75" s="9" t="str">
-        <f t="array" ref="H75">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B75,C75),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H75">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B75,C75),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I75" s="9" t="str">
         <f t="array" ref="I75">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B75,C75),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5690,12 +5694,12 @@
     </row>
     <row r="76" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B76" s="8">
-        <v>17.802979463</v>
-      </c>
-      <c r="C76" s="9">
-        <v>17.809999999999999</v>
-      </c>
-      <c r="D76" s="23" t="str">
+        <v>18.48</v>
+      </c>
+      <c r="C76" s="12">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="D76" s="12" t="str">
         <f t="shared" si="4"/>
         <v>-III</v>
       </c>
@@ -5712,8 +5716,8 @@
         <v>+III</v>
       </c>
       <c r="H76" s="9" t="str">
-        <f t="array" ref="H76">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B76,C76),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H76">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B76,C76),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I76" s="9" t="str">
         <f t="array" ref="I76">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B76,C76),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5734,12 +5738,12 @@
     </row>
     <row r="77" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B77" s="8">
-        <v>17.809999999999999</v>
-      </c>
-      <c r="C77" s="9">
-        <v>17.850000000000001</v>
-      </c>
-      <c r="D77" s="23" t="str">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="C77" s="12">
+        <v>18.57818717</v>
+      </c>
+      <c r="D77" s="12" t="str">
         <f t="shared" si="4"/>
         <v>-III</v>
       </c>
@@ -5756,8 +5760,8 @@
         <v>+III</v>
       </c>
       <c r="H77" s="9" t="str">
-        <f t="array" ref="H77">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B77,C77),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H77">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B77,C77),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>NR</v>
       </c>
       <c r="I77" s="9" t="str">
         <f t="array" ref="I77">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B77,C77),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5778,12 +5782,12 @@
     </row>
     <row r="78" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B78" s="8">
-        <v>17.850000000000001</v>
-      </c>
-      <c r="C78" s="9">
-        <v>17.91</v>
-      </c>
-      <c r="D78" s="23" t="str">
+        <v>18.57818717</v>
+      </c>
+      <c r="C78" s="12">
+        <v>18.588187170000001</v>
+      </c>
+      <c r="D78" s="12" t="str">
         <f t="shared" si="4"/>
         <v>-III</v>
       </c>
@@ -5800,8 +5804,8 @@
         <v>+III</v>
       </c>
       <c r="H78" s="9" t="str">
-        <f t="array" ref="H78">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B78,C78),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H78">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B78,C78),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>NR</v>
       </c>
       <c r="I78" s="9" t="str">
         <f t="array" ref="I78">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B78,C78),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5809,7 +5813,7 @@
       </c>
       <c r="J78" s="9" t="str">
         <f t="array" ref="J78">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B78,C78),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>NR</v>
+        <v>+III</v>
       </c>
       <c r="K78" s="9" t="str">
         <f t="array" ref="K78">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B78,C78),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
@@ -5822,12 +5826,12 @@
     </row>
     <row r="79" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B79" s="8">
-        <v>17.91</v>
-      </c>
-      <c r="C79" s="9">
-        <v>18.29</v>
-      </c>
-      <c r="D79" s="23" t="str">
+        <v>18.588187170000001</v>
+      </c>
+      <c r="C79" s="12">
+        <v>18.605671771000001</v>
+      </c>
+      <c r="D79" s="12" t="str">
         <f t="shared" si="4"/>
         <v>-III</v>
       </c>
@@ -5844,8 +5848,8 @@
         <v>+III</v>
       </c>
       <c r="H79" s="9" t="str">
-        <f t="array" ref="H79">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B79,C79),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H79">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B79,C79),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>NR</v>
       </c>
       <c r="I79" s="9" t="str">
         <f t="array" ref="I79">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B79,C79),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5866,30 +5870,30 @@
     </row>
     <row r="80" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B80" s="8">
-        <v>18.29</v>
-      </c>
-      <c r="C80" s="9">
-        <v>18.48</v>
-      </c>
-      <c r="D80" s="23" t="str">
+        <v>18.605671771000001</v>
+      </c>
+      <c r="C80" s="12">
+        <v>18.61409317</v>
+      </c>
+      <c r="D80" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>-III</v>
+        <v>+III</v>
       </c>
       <c r="E80" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>-III</v>
+        <v>+III</v>
       </c>
       <c r="F80" s="9" t="str">
         <f t="array" ref="F80">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B80,C80),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>-III</v>
+        <v>+III</v>
       </c>
       <c r="G80" s="9" t="str">
         <f t="array" ref="G80">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B80,C80),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="H80" s="9" t="str">
-        <f t="array" ref="H80">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B80,C80),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H80">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B80,C80),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>NR</v>
       </c>
       <c r="I80" s="9" t="str">
         <f t="array" ref="I80">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B80,C80),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5910,30 +5914,30 @@
     </row>
     <row r="81" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B81" s="8">
-        <v>18.48</v>
-      </c>
-      <c r="C81" s="9">
-        <v>18.559999999999999</v>
-      </c>
-      <c r="D81" s="23" t="str">
+        <v>18.61409317</v>
+      </c>
+      <c r="C81" s="12">
+        <v>18.624093169999998</v>
+      </c>
+      <c r="D81" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>-III</v>
+        <v>+II</v>
       </c>
       <c r="E81" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>-III</v>
+        <v>+II</v>
       </c>
       <c r="F81" s="9" t="str">
         <f t="array" ref="F81">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B81,C81),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>-III</v>
+        <v>+III</v>
       </c>
       <c r="G81" s="9" t="str">
         <f t="array" ref="G81">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B81,C81),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="H81" s="9" t="str">
-        <f t="array" ref="H81">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B81,C81),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H81">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B81,C81),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>NR</v>
       </c>
       <c r="I81" s="9" t="str">
         <f t="array" ref="I81">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B81,C81),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5941,43 +5945,43 @@
       </c>
       <c r="J81" s="9" t="str">
         <f t="array" ref="J81">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B81,C81),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>NR</v>
+        <v>+III</v>
       </c>
       <c r="K81" s="9" t="str">
         <f t="array" ref="K81">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B81,C81),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="L81" s="12" t="str">
         <f t="array" ref="L81">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B81,C81),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>NR</v>
+        <v>+III</v>
       </c>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B82" s="8">
-        <v>18.559999999999999</v>
-      </c>
-      <c r="C82" s="9">
-        <v>18.57818717</v>
-      </c>
-      <c r="D82" s="23" t="str">
+        <v>18.624093169999998</v>
+      </c>
+      <c r="C82" s="12">
+        <v>18.64</v>
+      </c>
+      <c r="D82" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>-III</v>
+        <v>+III</v>
       </c>
       <c r="E82" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>-III</v>
+        <v>+III</v>
       </c>
       <c r="F82" s="9" t="str">
         <f t="array" ref="F82">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B82,C82),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>-III</v>
+        <v>+III</v>
       </c>
       <c r="G82" s="9" t="str">
         <f t="array" ref="G82">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B82,C82),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="H82" s="9" t="str">
-        <f t="array" ref="H82">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B82,C82),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H82">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B82,C82),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>NR</v>
       </c>
       <c r="I82" s="9" t="str">
         <f t="array" ref="I82">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B82,C82),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -5998,30 +6002,30 @@
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B83" s="8">
-        <v>18.57818717</v>
-      </c>
-      <c r="C83" s="9">
-        <v>18.588187170000001</v>
-      </c>
-      <c r="D83" s="23" t="str">
+        <v>18.64</v>
+      </c>
+      <c r="C83" s="12">
+        <v>18.66</v>
+      </c>
+      <c r="D83" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>-III</v>
+        <v>+III</v>
       </c>
       <c r="E83" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>-III</v>
+        <v>+III</v>
       </c>
       <c r="F83" s="9" t="str">
         <f t="array" ref="F83">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B83,C83),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>-III</v>
+        <v>+III</v>
       </c>
       <c r="G83" s="9" t="str">
         <f t="array" ref="G83">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B83,C83),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="H83" s="9" t="str">
-        <f t="array" ref="H83">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B83,C83),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H83">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B83,C83),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I83" s="9" t="str">
         <f t="array" ref="I83">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B83,C83),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -6029,7 +6033,7 @@
       </c>
       <c r="J83" s="9" t="str">
         <f t="array" ref="J83">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B83,C83),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <v>NR</v>
       </c>
       <c r="K83" s="9" t="str">
         <f t="array" ref="K83">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B83,C83),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
@@ -6042,30 +6046,30 @@
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B84" s="8">
-        <v>18.588187170000001</v>
-      </c>
-      <c r="C84" s="9">
-        <v>18.605671771000001</v>
-      </c>
-      <c r="D84" s="23" t="str">
+        <v>18.66</v>
+      </c>
+      <c r="C84" s="12">
+        <v>18.75</v>
+      </c>
+      <c r="D84" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>-III</v>
+        <v>+III</v>
       </c>
       <c r="E84" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>-III</v>
+        <v>+III</v>
       </c>
       <c r="F84" s="9" t="str">
         <f t="array" ref="F84">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B84,C84),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>-III</v>
+        <v>+III</v>
       </c>
       <c r="G84" s="9" t="str">
         <f t="array" ref="G84">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B84,C84),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="H84" s="9" t="str">
-        <f t="array" ref="H84">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B84,C84),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H84">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B84,C84),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I84" s="9" t="str">
         <f t="array" ref="I84">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B84,C84),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -6086,18 +6090,18 @@
     </row>
     <row r="85" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B85" s="8">
-        <v>18.605671771000001</v>
-      </c>
-      <c r="C85" s="9">
-        <v>18.605671772000001</v>
-      </c>
-      <c r="D85" s="23" t="str">
+        <v>18.75</v>
+      </c>
+      <c r="C85" s="12">
+        <v>19.070850830000001</v>
+      </c>
+      <c r="D85" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="E85" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="F85" s="9" t="str">
         <f t="array" ref="F85">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B85,C85),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
@@ -6108,8 +6112,8 @@
         <v>+III</v>
       </c>
       <c r="H85" s="9" t="str">
-        <f t="array" ref="H85">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B85,C85),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H85">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B85,C85),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>NR</v>
       </c>
       <c r="I85" s="9" t="str">
         <f t="array" ref="I85">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B85,C85),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -6130,18 +6134,18 @@
     </row>
     <row r="86" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B86" s="8">
-        <v>18.605671772000001</v>
-      </c>
-      <c r="C86" s="9">
-        <v>18.61409317</v>
-      </c>
-      <c r="D86" s="23" t="str">
+        <v>19.070850830000001</v>
+      </c>
+      <c r="C86" s="12">
+        <v>19.080850829999999</v>
+      </c>
+      <c r="D86" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>+II</v>
+        <v>+I</v>
       </c>
       <c r="E86" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>+II</v>
+        <v>+I</v>
       </c>
       <c r="F86" s="9" t="str">
         <f t="array" ref="F86">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B86,C86),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
@@ -6152,8 +6156,8 @@
         <v>+III</v>
       </c>
       <c r="H86" s="9" t="str">
-        <f t="array" ref="H86">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B86,C86),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H86">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B86,C86),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>NR</v>
       </c>
       <c r="I86" s="9" t="str">
         <f t="array" ref="I86">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B86,C86),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -6161,11 +6165,11 @@
       </c>
       <c r="J86" s="9" t="str">
         <f t="array" ref="J86">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B86,C86),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>NR</v>
+        <v>+I</v>
       </c>
       <c r="K86" s="9" t="str">
         <f t="array" ref="K86">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B86,C86),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="L86" s="12" t="str">
         <f t="array" ref="L86">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B86,C86),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
@@ -6174,18 +6178,18 @@
     </row>
     <row r="87" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B87" s="8">
-        <v>18.61409317</v>
-      </c>
-      <c r="C87" s="9">
-        <v>18.624093169999998</v>
-      </c>
-      <c r="D87" s="23" t="str">
+        <v>19.080850829999999</v>
+      </c>
+      <c r="C87" s="12">
+        <v>19.13233735</v>
+      </c>
+      <c r="D87" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="E87" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="F87" s="9" t="str">
         <f t="array" ref="F87">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B87,C87),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
@@ -6196,8 +6200,8 @@
         <v>+III</v>
       </c>
       <c r="H87" s="9" t="str">
-        <f t="array" ref="H87">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B87,C87),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H87">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B87,C87),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>NR</v>
       </c>
       <c r="I87" s="9" t="str">
         <f t="array" ref="I87">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B87,C87),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -6205,31 +6209,31 @@
       </c>
       <c r="J87" s="9" t="str">
         <f t="array" ref="J87">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B87,C87),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <v>NR</v>
       </c>
       <c r="K87" s="9" t="str">
         <f t="array" ref="K87">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B87,C87),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="L87" s="12" t="str">
         <f t="array" ref="L87">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B87,C87),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <v>NR</v>
       </c>
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B88" s="8">
-        <v>18.624093169999998</v>
-      </c>
-      <c r="C88" s="9">
-        <v>18.64</v>
-      </c>
-      <c r="D88" s="23" t="str">
+        <v>19.13233735</v>
+      </c>
+      <c r="C88" s="12">
+        <v>19.142337349999998</v>
+      </c>
+      <c r="D88" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="E88" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="F88" s="9" t="str">
         <f t="array" ref="F88">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B88,C88),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
@@ -6240,8 +6244,8 @@
         <v>+III</v>
       </c>
       <c r="H88" s="9" t="str">
-        <f t="array" ref="H88">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B88,C88),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H88">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B88,C88),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>NR</v>
       </c>
       <c r="I88" s="9" t="str">
         <f t="array" ref="I88">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B88,C88),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -6249,7 +6253,7 @@
       </c>
       <c r="J88" s="9" t="str">
         <f t="array" ref="J88">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B88,C88),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>NR</v>
+        <v>+III</v>
       </c>
       <c r="K88" s="9" t="str">
         <f t="array" ref="K88">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B88,C88),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
@@ -6262,18 +6266,18 @@
     </row>
     <row r="89" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B89" s="8">
-        <v>18.64</v>
-      </c>
-      <c r="C89" s="9">
-        <v>18.66</v>
-      </c>
-      <c r="D89" s="23" t="str">
+        <v>19.142337349999998</v>
+      </c>
+      <c r="C89" s="12">
+        <v>19.574514854</v>
+      </c>
+      <c r="D89" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="E89" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="F89" s="9" t="str">
         <f t="array" ref="F89">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B89,C89),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
@@ -6284,8 +6288,8 @@
         <v>+III</v>
       </c>
       <c r="H89" s="9" t="str">
-        <f t="array" ref="H89">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B89,C89),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H89">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B89,C89),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>NR</v>
       </c>
       <c r="I89" s="9" t="str">
         <f t="array" ref="I89">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B89,C89),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -6306,18 +6310,18 @@
     </row>
     <row r="90" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B90" s="8">
-        <v>18.66</v>
-      </c>
-      <c r="C90" s="9">
-        <v>18.75</v>
-      </c>
-      <c r="D90" s="23" t="str">
+        <v>19.574514854</v>
+      </c>
+      <c r="C90" s="12">
+        <v>19.670000000000002</v>
+      </c>
+      <c r="D90" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="E90" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="F90" s="9" t="str">
         <f t="array" ref="F90">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B90,C90),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
@@ -6328,8 +6332,8 @@
         <v>+III</v>
       </c>
       <c r="H90" s="9" t="str">
-        <f t="array" ref="H90">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B90,C90),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H90">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B90,C90),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>NR</v>
       </c>
       <c r="I90" s="9" t="str">
         <f t="array" ref="I90">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B90,C90),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -6350,18 +6354,18 @@
     </row>
     <row r="91" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B91" s="8">
-        <v>18.75</v>
-      </c>
-      <c r="C91" s="9">
-        <v>19.070850830000001</v>
-      </c>
-      <c r="D91" s="23" t="str">
+        <v>19.670000000000002</v>
+      </c>
+      <c r="C91" s="12">
+        <v>19.69841048</v>
+      </c>
+      <c r="D91" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="E91" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="F91" s="9" t="str">
         <f t="array" ref="F91">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B91,C91),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
@@ -6372,8 +6376,8 @@
         <v>+III</v>
       </c>
       <c r="H91" s="9" t="str">
-        <f t="array" ref="H91">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B91,C91),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H91">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B91,C91),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I91" s="9" t="str">
         <f t="array" ref="I91">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B91,C91),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -6394,18 +6398,18 @@
     </row>
     <row r="92" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B92" s="8">
-        <v>19.070850830000001</v>
-      </c>
-      <c r="C92" s="9">
-        <v>19.080850829999999</v>
-      </c>
-      <c r="D92" s="23" t="str">
+        <v>19.69841048</v>
+      </c>
+      <c r="C92" s="12">
+        <v>19.809999999999999</v>
+      </c>
+      <c r="D92" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>+I</v>
+        <v>+III</v>
       </c>
       <c r="E92" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>+I</v>
+        <v>+III</v>
       </c>
       <c r="F92" s="9" t="str">
         <f t="array" ref="F92">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B92,C92),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
@@ -6416,8 +6420,8 @@
         <v>+III</v>
       </c>
       <c r="H92" s="9" t="str">
-        <f t="array" ref="H92">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B92,C92),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H92">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B92,C92),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I92" s="9" t="str">
         <f t="array" ref="I92">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B92,C92),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -6425,11 +6429,11 @@
       </c>
       <c r="J92" s="9" t="str">
         <f t="array" ref="J92">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B92,C92),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+I</v>
+        <v>NR</v>
       </c>
       <c r="K92" s="9" t="str">
         <f t="array" ref="K92">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B92,C92),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="L92" s="12" t="str">
         <f t="array" ref="L92">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B92,C92),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
@@ -6438,18 +6442,18 @@
     </row>
     <row r="93" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B93" s="8">
-        <v>19.080850829999999</v>
-      </c>
-      <c r="C93" s="9">
-        <v>19.13233735</v>
-      </c>
-      <c r="D93" s="23" t="str">
+        <v>19.809999999999999</v>
+      </c>
+      <c r="C93" s="12">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="D93" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="E93" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="F93" s="9" t="str">
         <f t="array" ref="F93">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B93,C93),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
@@ -6460,8 +6464,8 @@
         <v>+III</v>
       </c>
       <c r="H93" s="9" t="str">
-        <f t="array" ref="H93">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B93,C93),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H93">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B93,C93),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I93" s="9" t="str">
         <f t="array" ref="I93">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B93,C93),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -6482,18 +6486,18 @@
     </row>
     <row r="94" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B94" s="8">
-        <v>19.13233735</v>
-      </c>
-      <c r="C94" s="9">
-        <v>19.142337349999998</v>
-      </c>
-      <c r="D94" s="23" t="str">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="C94" s="12">
+        <v>20.352428100000001</v>
+      </c>
+      <c r="D94" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="E94" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="F94" s="9" t="str">
         <f t="array" ref="F94">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B94,C94),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
@@ -6504,8 +6508,8 @@
         <v>+III</v>
       </c>
       <c r="H94" s="9" t="str">
-        <f t="array" ref="H94">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B94,C94),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H94">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B94,C94),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I94" s="9" t="str">
         <f t="array" ref="I94">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B94,C94),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -6513,7 +6517,7 @@
       </c>
       <c r="J94" s="9" t="str">
         <f t="array" ref="J94">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B94,C94),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <v>NR</v>
       </c>
       <c r="K94" s="9" t="str">
         <f t="array" ref="K94">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B94,C94),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
@@ -6526,18 +6530,18 @@
     </row>
     <row r="95" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B95" s="8">
-        <v>19.142337349999998</v>
-      </c>
-      <c r="C95" s="9">
-        <v>19.574514854</v>
-      </c>
-      <c r="D95" s="23" t="str">
+        <v>20.352428100000001</v>
+      </c>
+      <c r="C95" s="12">
+        <v>20.362428099999999</v>
+      </c>
+      <c r="D95" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="E95" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="F95" s="9" t="str">
         <f t="array" ref="F95">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B95,C95),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
@@ -6548,8 +6552,8 @@
         <v>+III</v>
       </c>
       <c r="H95" s="9" t="str">
-        <f t="array" ref="H95">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B95,C95),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H95">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B95,C95),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I95" s="9" t="str">
         <f t="array" ref="I95">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B95,C95),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -6557,7 +6561,7 @@
       </c>
       <c r="J95" s="9" t="str">
         <f t="array" ref="J95">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B95,C95),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>NR</v>
+        <v>+III</v>
       </c>
       <c r="K95" s="9" t="str">
         <f t="array" ref="K95">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B95,C95),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
@@ -6570,18 +6574,18 @@
     </row>
     <row r="96" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B96" s="8">
-        <v>19.574514854</v>
-      </c>
-      <c r="C96" s="9">
-        <v>19.670000000000002</v>
-      </c>
-      <c r="D96" s="23" t="str">
+        <v>20.362428099999999</v>
+      </c>
+      <c r="C96" s="12">
+        <v>20.49</v>
+      </c>
+      <c r="D96" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="E96" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="F96" s="9" t="str">
         <f t="array" ref="F96">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B96,C96),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
@@ -6592,8 +6596,8 @@
         <v>+III</v>
       </c>
       <c r="H96" s="9" t="str">
-        <f t="array" ref="H96">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B96,C96),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H96">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B96,C96),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I96" s="9" t="str">
         <f t="array" ref="I96">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B96,C96),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -6614,18 +6618,18 @@
     </row>
     <row r="97" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B97" s="8">
-        <v>19.670000000000002</v>
-      </c>
-      <c r="C97" s="9">
-        <v>19.69841048</v>
-      </c>
-      <c r="D97" s="23" t="str">
+        <v>20.49</v>
+      </c>
+      <c r="C97" s="12">
+        <v>20.64</v>
+      </c>
+      <c r="D97" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="E97" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="F97" s="9" t="str">
         <f t="array" ref="F97">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B97,C97),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
@@ -6636,8 +6640,8 @@
         <v>+III</v>
       </c>
       <c r="H97" s="9" t="str">
-        <f t="array" ref="H97">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B97,C97),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H97">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B97,C97),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I97" s="9" t="str">
         <f t="array" ref="I97">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B97,C97),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -6658,18 +6662,18 @@
     </row>
     <row r="98" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B98" s="8">
-        <v>19.69841048</v>
-      </c>
-      <c r="C98" s="9">
-        <v>19.809999999999999</v>
-      </c>
-      <c r="D98" s="23" t="str">
+        <v>20.64</v>
+      </c>
+      <c r="C98" s="12">
+        <v>20.69</v>
+      </c>
+      <c r="D98" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="E98" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="F98" s="9" t="str">
         <f t="array" ref="F98">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B98,C98),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
@@ -6680,8 +6684,8 @@
         <v>+III</v>
       </c>
       <c r="H98" s="9" t="str">
-        <f t="array" ref="H98">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B98,C98),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H98">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B98,C98),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I98" s="9" t="str">
         <f t="array" ref="I98">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B98,C98),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -6702,18 +6706,18 @@
     </row>
     <row r="99" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B99" s="8">
-        <v>19.809999999999999</v>
-      </c>
-      <c r="C99" s="9">
-        <v>19.989999999999998</v>
-      </c>
-      <c r="D99" s="23" t="str">
-        <f t="shared" ref="D99:D106" si="6">IF(COUNTIF(F99:L99,"D")&gt;0,"D",IF(COUNTIF(F99:L99,"-III")&gt;0,"-III",IF(COUNTIF(F99:L99,"-II")&gt;0,"-II",IF(COUNTIF(F99:L99,"-I")&gt;0,"-I",IF(COUNTIF(F99:L99,"+0")&gt;0,"+0",IF(COUNTIF(F99:L99,"+I")&gt;0,"+I",IF(COUNTIF(F99:L99,"+II")&gt;0,"+II",IF(COUNTIF(F99:L99,"+III")&gt;0,"+III",IF(COUNTIF(F99:L99,"ND")&gt;0,"ND","NR")))))))))</f>
-        <v>+II</v>
+        <v>20.69</v>
+      </c>
+      <c r="C99" s="12">
+        <v>20.76</v>
+      </c>
+      <c r="D99" s="12" t="str">
+        <f t="shared" ref="D99" si="6">IF(COUNTIF(F99:L99,"D")&gt;0,"D",IF(COUNTIF(F99:L99,"-III")&gt;0,"-III",IF(COUNTIF(F99:L99,"-II")&gt;0,"-II",IF(COUNTIF(F99:L99,"-I")&gt;0,"-I",IF(COUNTIF(F99:L99,"+0")&gt;0,"+0",IF(COUNTIF(F99:L99,"+I")&gt;0,"+I",IF(COUNTIF(F99:L99,"+II")&gt;0,"+II",IF(COUNTIF(F99:L99,"+III")&gt;0,"+III",IF(COUNTIF(F99:L99,"ND")&gt;0,"ND","NR")))))))))</f>
+        <v>+III</v>
       </c>
       <c r="E99" s="23" t="str">
-        <f t="shared" ref="E99:E106" si="7">IF(COUNTIF(F99:L99,"-III")&gt;0,"-III",IF(COUNTIF(F99:L99,"-II")&gt;0,"-II",IF(COUNTIF(F99:L99,"-I")&gt;0,"-I",IF(COUNTIF(F99:L99,"+0")&gt;0,"+0",IF(COUNTIF(F99:L99,"+I")&gt;0,"+I",IF(COUNTIF(F99:L99,"+II")&gt;0,"+II",IF(COUNTIF(F99:L99,"+III")&gt;0,"+III",IF(COUNTIF(F99:L99,"ND")&gt;0,"ND","NR"))))))))</f>
-        <v>+II</v>
+        <f t="shared" ref="E99" si="7">IF(COUNTIF(F99:L99,"-III")&gt;0,"-III",IF(COUNTIF(F99:L99,"-II")&gt;0,"-II",IF(COUNTIF(F99:L99,"-I")&gt;0,"-I",IF(COUNTIF(F99:L99,"+0")&gt;0,"+0",IF(COUNTIF(F99:L99,"+I")&gt;0,"+I",IF(COUNTIF(F99:L99,"+II")&gt;0,"+II",IF(COUNTIF(F99:L99,"+III")&gt;0,"+III",IF(COUNTIF(F99:L99,"ND")&gt;0,"ND","NR"))))))))</f>
+        <v>+III</v>
       </c>
       <c r="F99" s="9" t="str">
         <f t="array" ref="F99">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B99,C99),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
@@ -6724,8 +6728,8 @@
         <v>+III</v>
       </c>
       <c r="H99" s="9" t="str">
-        <f t="array" ref="H99">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B99,C99),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H99">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B99,C99),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I99" s="9" t="str">
         <f t="array" ref="I99">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B99,C99),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -6746,18 +6750,18 @@
     </row>
     <row r="100" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B100" s="8">
-        <v>19.989999999999998</v>
+        <v>20.76</v>
       </c>
       <c r="C100" s="9">
-        <v>20.352428100000001</v>
-      </c>
-      <c r="D100" s="23" t="str">
-        <f t="shared" si="6"/>
-        <v>+II</v>
+        <v>20.93</v>
+      </c>
+      <c r="D100" s="12" t="str">
+        <f t="shared" ref="D100" si="8">IF(COUNTIF(F100:L100,"D")&gt;0,"D",IF(COUNTIF(F100:L100,"-III")&gt;0,"-III",IF(COUNTIF(F100:L100,"-II")&gt;0,"-II",IF(COUNTIF(F100:L100,"-I")&gt;0,"-I",IF(COUNTIF(F100:L100,"+0")&gt;0,"+0",IF(COUNTIF(F100:L100,"+I")&gt;0,"+I",IF(COUNTIF(F100:L100,"+II")&gt;0,"+II",IF(COUNTIF(F100:L100,"+III")&gt;0,"+III",IF(COUNTIF(F100:L100,"ND")&gt;0,"ND","NR")))))))))</f>
+        <v>+III</v>
       </c>
       <c r="E100" s="23" t="str">
-        <f t="shared" si="7"/>
-        <v>+II</v>
+        <f t="shared" ref="E100" si="9">IF(COUNTIF(F100:L100,"-III")&gt;0,"-III",IF(COUNTIF(F100:L100,"-II")&gt;0,"-II",IF(COUNTIF(F100:L100,"-I")&gt;0,"-I",IF(COUNTIF(F100:L100,"+0")&gt;0,"+0",IF(COUNTIF(F100:L100,"+I")&gt;0,"+I",IF(COUNTIF(F100:L100,"+II")&gt;0,"+II",IF(COUNTIF(F100:L100,"+III")&gt;0,"+III",IF(COUNTIF(F100:L100,"ND")&gt;0,"ND","NR"))))))))</f>
+        <v>+III</v>
       </c>
       <c r="F100" s="9" t="str">
         <f t="array" ref="F100">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B100,C100),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
@@ -6768,8 +6772,8 @@
         <v>+III</v>
       </c>
       <c r="H100" s="9" t="str">
-        <f t="array" ref="H100">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B100,C100),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
+        <f t="array" ref="H100">INDEX(GEKB!$K$11:$K$100,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$100&gt;AVERAGE(B100,C100),GEKB!$D$11:$D$100)),GEKB!$D$11:$D$100),1))</f>
+        <v>+III</v>
       </c>
       <c r="I100" s="9" t="str">
         <f t="array" ref="I100">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B100,C100),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
@@ -6789,268 +6793,82 @@
       </c>
     </row>
     <row r="101" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B101" s="8">
-        <v>20.352428100000001</v>
-      </c>
-      <c r="C101" s="9">
-        <v>20.362428099999999</v>
-      </c>
-      <c r="D101" s="23" t="str">
-        <f t="shared" si="6"/>
-        <v>+II</v>
-      </c>
-      <c r="E101" s="23" t="str">
-        <f t="shared" si="7"/>
-        <v>+II</v>
-      </c>
-      <c r="F101" s="9" t="str">
-        <f t="array" ref="F101">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B101,C101),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="G101" s="9" t="str">
-        <f t="array" ref="G101">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B101,C101),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H101" s="9" t="str">
-        <f t="array" ref="H101">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B101,C101),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="I101" s="9" t="str">
-        <f t="array" ref="I101">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B101,C101),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="J101" s="9" t="str">
-        <f t="array" ref="J101">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B101,C101),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K101" s="9" t="str">
-        <f t="array" ref="K101">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B101,C101),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="L101" s="12" t="str">
-        <f t="array" ref="L101">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B101,C101),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
+      <c r="B101" s="8"/>
+      <c r="C101" s="12"/>
+      <c r="D101" s="12"/>
+      <c r="E101" s="23"/>
+      <c r="F101" s="9"/>
+      <c r="G101" s="9"/>
+      <c r="H101" s="9"/>
+      <c r="I101" s="9"/>
+      <c r="J101" s="9"/>
+      <c r="K101" s="9"/>
+      <c r="L101" s="12"/>
     </row>
     <row r="102" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B102" s="8">
-        <v>20.362428099999999</v>
-      </c>
-      <c r="C102" s="9">
-        <v>20.49</v>
-      </c>
-      <c r="D102" s="23" t="str">
-        <f t="shared" si="6"/>
-        <v>+II</v>
-      </c>
-      <c r="E102" s="23" t="str">
-        <f t="shared" si="7"/>
-        <v>+II</v>
-      </c>
-      <c r="F102" s="9" t="str">
-        <f t="array" ref="F102">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B102,C102),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="G102" s="9" t="str">
-        <f t="array" ref="G102">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B102,C102),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H102" s="9" t="str">
-        <f t="array" ref="H102">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B102,C102),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="I102" s="9" t="str">
-        <f t="array" ref="I102">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B102,C102),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="J102" s="9" t="str">
-        <f t="array" ref="J102">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B102,C102),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="K102" s="9" t="str">
-        <f t="array" ref="K102">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B102,C102),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="L102" s="12" t="str">
-        <f t="array" ref="L102">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B102,C102),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
+      <c r="B102" s="8"/>
+      <c r="C102" s="12"/>
+      <c r="D102" s="12"/>
+      <c r="E102" s="23"/>
+      <c r="F102" s="9"/>
+      <c r="G102" s="9"/>
+      <c r="H102" s="9"/>
+      <c r="I102" s="9"/>
+      <c r="J102" s="9"/>
+      <c r="K102" s="9"/>
+      <c r="L102" s="12"/>
     </row>
     <row r="103" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B103" s="8">
-        <v>20.49</v>
-      </c>
-      <c r="C103" s="9">
-        <v>20.64</v>
-      </c>
-      <c r="D103" s="23" t="str">
-        <f t="shared" si="6"/>
-        <v>+II</v>
-      </c>
-      <c r="E103" s="23" t="str">
-        <f t="shared" si="7"/>
-        <v>+II</v>
-      </c>
-      <c r="F103" s="9" t="str">
-        <f t="array" ref="F103">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B103,C103),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="G103" s="9" t="str">
-        <f t="array" ref="G103">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B103,C103),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H103" s="9" t="str">
-        <f t="array" ref="H103">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B103,C103),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="I103" s="9" t="str">
-        <f t="array" ref="I103">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B103,C103),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="J103" s="9" t="str">
-        <f t="array" ref="J103">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B103,C103),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="K103" s="9" t="str">
-        <f t="array" ref="K103">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B103,C103),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="L103" s="12" t="str">
-        <f t="array" ref="L103">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B103,C103),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
+      <c r="B103" s="8"/>
+      <c r="C103" s="12"/>
+      <c r="D103" s="12"/>
+      <c r="E103" s="23"/>
+      <c r="F103" s="9"/>
+      <c r="G103" s="9"/>
+      <c r="H103" s="9"/>
+      <c r="I103" s="9"/>
+      <c r="J103" s="9"/>
+      <c r="K103" s="9"/>
+      <c r="L103" s="12"/>
     </row>
     <row r="104" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B104" s="8">
-        <v>20.64</v>
-      </c>
-      <c r="C104" s="9">
-        <v>20.69</v>
-      </c>
-      <c r="D104" s="23" t="str">
-        <f t="shared" si="6"/>
-        <v>+II</v>
-      </c>
-      <c r="E104" s="23" t="str">
-        <f t="shared" si="7"/>
-        <v>+II</v>
-      </c>
-      <c r="F104" s="9" t="str">
-        <f t="array" ref="F104">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B104,C104),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="G104" s="9" t="str">
-        <f t="array" ref="G104">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B104,C104),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H104" s="9" t="str">
-        <f t="array" ref="H104">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B104,C104),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="I104" s="9" t="str">
-        <f t="array" ref="I104">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B104,C104),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="J104" s="9" t="str">
-        <f t="array" ref="J104">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B104,C104),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="K104" s="9" t="str">
-        <f t="array" ref="K104">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B104,C104),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="L104" s="12" t="str">
-        <f t="array" ref="L104">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B104,C104),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
+      <c r="B104" s="8"/>
+      <c r="C104" s="12"/>
+      <c r="D104" s="12"/>
+      <c r="E104" s="23"/>
+      <c r="F104" s="9"/>
+      <c r="G104" s="9"/>
+      <c r="H104" s="9"/>
+      <c r="I104" s="9"/>
+      <c r="J104" s="9"/>
+      <c r="K104" s="9"/>
+      <c r="L104" s="12"/>
     </row>
     <row r="105" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B105" s="8">
-        <v>20.69</v>
-      </c>
-      <c r="C105" s="9">
-        <v>20.76</v>
-      </c>
-      <c r="D105" s="23" t="str">
-        <f t="shared" si="6"/>
-        <v>+II</v>
-      </c>
-      <c r="E105" s="23" t="str">
-        <f t="shared" si="7"/>
-        <v>+II</v>
-      </c>
-      <c r="F105" s="9" t="str">
-        <f t="array" ref="F105">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B105,C105),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="G105" s="9" t="str">
-        <f t="array" ref="G105">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B105,C105),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H105" s="9" t="str">
-        <f t="array" ref="H105">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B105,C105),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="I105" s="9" t="str">
-        <f t="array" ref="I105">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B105,C105),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="J105" s="9" t="str">
-        <f t="array" ref="J105">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B105,C105),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="K105" s="9" t="str">
-        <f t="array" ref="K105">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B105,C105),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="L105" s="12" t="str">
-        <f t="array" ref="L105">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B105,C105),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
+      <c r="B105" s="8"/>
+      <c r="C105" s="12"/>
+      <c r="D105" s="12"/>
+      <c r="E105" s="23"/>
+      <c r="F105" s="9"/>
+      <c r="G105" s="9"/>
+      <c r="H105" s="9"/>
+      <c r="I105" s="9"/>
+      <c r="J105" s="9"/>
+      <c r="K105" s="9"/>
+      <c r="L105" s="12"/>
     </row>
     <row r="106" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="13">
-        <v>20.76</v>
-      </c>
-      <c r="C106" s="14">
-        <v>20.93</v>
-      </c>
-      <c r="D106" s="24" t="str">
-        <f t="shared" si="6"/>
-        <v>+II</v>
-      </c>
-      <c r="E106" s="24" t="str">
-        <f t="shared" si="7"/>
-        <v>+II</v>
-      </c>
-      <c r="F106" s="14" t="str">
-        <f t="array" ref="F106">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B106,C106),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="G106" s="14" t="str">
-        <f t="array" ref="G106">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B106,C106),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H106" s="14" t="str">
-        <f t="array" ref="H106">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B106,C106),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="I106" s="14" t="str">
-        <f t="array" ref="I106">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B106,C106),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="J106" s="14" t="str">
-        <f t="array" ref="J106">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B106,C106),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="K106" s="14" t="str">
-        <f t="array" ref="K106">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B106,C106),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="L106" s="17" t="str">
-        <f t="array" ref="L106">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B106,C106),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
+      <c r="B106" s="13"/>
+      <c r="C106" s="17"/>
+      <c r="D106" s="17"/>
+      <c r="E106" s="24"/>
+      <c r="F106" s="14"/>
+      <c r="G106" s="14"/>
+      <c r="H106" s="14"/>
+      <c r="I106" s="14"/>
+      <c r="J106" s="14"/>
+      <c r="K106" s="14"/>
+      <c r="L106" s="17"/>
     </row>
     <row r="107" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B107" s="9"/>
@@ -7141,9 +6959,6 @@
       <c r="C135" s="9"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C136">
-    <sortCondition ref="B2:B136"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -7154,7 +6969,7 @@
   <dimension ref="A2:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10759,8 +10574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E4BDF32-8A22-4A66-B6B5-DB37648E7DC4}">
   <dimension ref="B2:U73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ASK-41 Implement Test for correct assessment grade
</commit_message>
<xml_diff>
--- a/benchmarktests/testdefinitions/Benchmarktest_traject 12-2.xlsx
+++ b/benchmarktests/testdefinitions/Benchmarktest_traject 12-2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993D2AB8-A2A2-4CF2-BB57-D9BD80419B16}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D220E3D-D4DE-4D29-B9AE-64B7EF9BDB80}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="653" firstSheet="1" activeTab="2" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="653" firstSheet="1" activeTab="9" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
   </bookViews>
   <sheets>
     <sheet name="Informatiepagina" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="183">
   <si>
     <t>Vaknaam</t>
   </si>
@@ -2125,8 +2125,8 @@
   </sheetPr>
   <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2141,20 +2141,20 @@
         <v>84</v>
       </c>
       <c r="D2" s="1">
-        <f>IFERROR(1-PRODUCT(G7:G12),"GR")</f>
-        <v>6.0685267360869544E-2</v>
+        <f>IFERROR(1-PRODUCT(G7:G14),"GR")</f>
+        <v>6.0686446349930367E-2</v>
       </c>
       <c r="E2" t="str">
         <f>IF(D2="GR","-",INDEX('Normen en duidingsklassen'!$D$4:$D$8,H2))</f>
-        <v>A+</v>
+        <v>D</v>
       </c>
       <c r="G2">
-        <f t="array" ref="G2">MIN(IF('Normen en duidingsklassen'!$F$4:$F$8&gt;D2,'Normen en duidingsklassen'!$F$4:$F$8))</f>
-        <v>0</v>
+        <f t="array" ref="G2">MIN(IF('Normen en duidingsklassen'!$E$4:$E$8&gt;=D2,'Normen en duidingsklassen'!$F$4:$F$8))</f>
+        <v>0.03</v>
       </c>
       <c r="H2">
-        <f>IFERROR(MATCH(G2,'Normen en duidingsklassen'!$F$4:$F$8),1)</f>
-        <v>1</v>
+        <f>IFERROR(MATCH(G2,'Normen en duidingsklassen'!$F$4:$F$8,0),1)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -2162,20 +2162,20 @@
         <v>83</v>
       </c>
       <c r="D3" s="1">
-        <f>1-PRODUCT(H7:H12)</f>
-        <v>6.0685267360869544E-2</v>
+        <f>1-PRODUCT(H7:H14)</f>
+        <v>6.0686446349930367E-2</v>
       </c>
       <c r="E3" t="str">
         <f>INDEX('Normen en duidingsklassen'!$D$4:$D$8,H3)</f>
-        <v>A+</v>
+        <v>D</v>
       </c>
       <c r="G3">
-        <f t="array" ref="G3">MIN(IF('Normen en duidingsklassen'!$F$4:$F$8&gt;D3,'Normen en duidingsklassen'!$F$4:$F$8))</f>
-        <v>0</v>
+        <f t="array" ref="G3">MIN(IF('Normen en duidingsklassen'!$E$4:$E$8&gt;=D3,'Normen en duidingsklassen'!$F$4:$F$8))</f>
+        <v>0.03</v>
       </c>
       <c r="H3">
         <f>IFERROR(MATCH(G3,'Normen en duidingsklassen'!$F$4:$F$8),1)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2237,11 +2237,11 @@
       </c>
       <c r="E8" s="49"/>
       <c r="G8" s="1">
-        <f t="shared" ref="G8:G14" si="0">IF(ISNUMBER(E8),1-E8,1-C8)</f>
+        <f t="shared" ref="G8:G13" si="0">IF(ISNUMBER(E8),1-E8,1-C8)</f>
         <v>0.99999625083543664</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" ref="H8:H14" si="1">IF(ISNUMBER(E8),1-E8,1-D8)</f>
+        <f t="shared" ref="H8:H13" si="1">IF(ISNUMBER(E8),1-E8,1-D8)</f>
         <v>0.99999625083543664</v>
       </c>
     </row>
@@ -2334,17 +2334,25 @@
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="40"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="26"/>
+      <c r="B13" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="31">
+        <f>BSKW!C5</f>
+        <v>1.2551587022663145E-6</v>
+      </c>
+      <c r="D13" s="26">
+        <f>BSKW!C6</f>
+        <v>1.2551587022663145E-6</v>
+      </c>
       <c r="E13" s="49"/>
       <c r="G13" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.99999874484129769</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.99999874484129769</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2352,14 +2360,8 @@
       <c r="C14" s="33"/>
       <c r="D14" s="27"/>
       <c r="E14" s="51"/>
-      <c r="G14" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H14" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7202,7 +7204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49710E67-B736-4749-B620-06835F5DE469}">
   <dimension ref="B2:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -17299,7 +17301,7 @@
   <dimension ref="B2:U29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>